<commit_message>
Actualización Toggl Diego desde mayo 20 a junio 7
</commit_message>
<xml_diff>
--- a/MEJORA_CONTINUA/VERSIÓN INICIAL V2.xlsx
+++ b/MEJORA_CONTINUA/VERSIÓN INICIAL V2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\REPOSITORIO_PROYECTOS\GESTION-CALIDAD-ANALITICA\MEJORA_CONTINUA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\REPOSITORIOS_ANALITICA\PROD\GESTION-CALIDAD-ANALITICA\MEJORA_CONTINUA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9135" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DESCRIPCIÓN" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="127">
   <si>
     <t>Workspace</t>
   </si>
@@ -272,6 +272,147 @@
   </si>
   <si>
     <t>2019-06-03 - 2019-06-09</t>
+  </si>
+  <si>
+    <t>Auditoria</t>
+  </si>
+  <si>
+    <t>Plan de intervención del programa de riesgo psicosocial</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>PROYECTO 1. MEJORAS FACTURACIÓN</t>
+  </si>
+  <si>
+    <t>Mejora para que las ediciones de factura se visualicen en el adjunto exportado</t>
+  </si>
+  <si>
+    <t>Actualización mejora para edit factura</t>
+  </si>
+  <si>
+    <t>PROYECTO 4. PILOTO APRENDIZ FORMATOS</t>
+  </si>
+  <si>
+    <t>Seguimiento Cinecolombia</t>
+  </si>
+  <si>
+    <t>PROYECTO 5. CALIFICACIÓN CONTRATISTAS</t>
+  </si>
+  <si>
+    <t>Mejora permisos</t>
+  </si>
+  <si>
+    <t>Mejora popup de usuario</t>
+  </si>
+  <si>
+    <t>Incluir el nombre del CECO en el buscador de los indicadores financieras</t>
+  </si>
+  <si>
+    <t>Maqueta y flujo app registro contratistas</t>
+  </si>
+  <si>
+    <t>Compromiso comunidad de control</t>
+  </si>
+  <si>
+    <t>Weekly</t>
+  </si>
+  <si>
+    <t>REUNION PLANIFICACION</t>
+  </si>
+  <si>
+    <t>Corrección R para que no se borren las facturas creadas en un mismo mes</t>
+  </si>
+  <si>
+    <t>Muestra del Div de total personas y Merge de mejoras</t>
+  </si>
+  <si>
+    <t>Revision error vista edición flujo de proyectos</t>
+  </si>
+  <si>
+    <t>Corrección error de flow de creacion de actividades precedentes</t>
+  </si>
+  <si>
+    <t>Corrección de usuarios y loggin</t>
+  </si>
+  <si>
+    <t>Corrección de vista detalles registro calificaciones</t>
+  </si>
+  <si>
+    <t>Entrega CONTRATISTAS módulo calificaciones</t>
+  </si>
+  <si>
+    <t>Evaluación de cambio de la vista de revisión de calificaciones</t>
+  </si>
+  <si>
+    <t>Mejora vista revisiones</t>
+  </si>
+  <si>
+    <t>Pruebas y mejora de la VISTA_DETALLES_REGISTROS_CALIFICACIONES_CHILD para mostrar por orden de fechas</t>
+  </si>
+  <si>
+    <t>Ajustar URL de descarga</t>
+  </si>
+  <si>
+    <t>Documentación carga archivo indicadores en servidor</t>
+  </si>
+  <si>
+    <t>Revisión de reporte de indicadores de gestión</t>
+  </si>
+  <si>
+    <t>Revision requerimiento INDICADORES - TIPO DE SERVICIO</t>
+  </si>
+  <si>
+    <t>ALMUERZO</t>
+  </si>
+  <si>
+    <t>Reunión comunidad de control</t>
+  </si>
+  <si>
+    <t>RECEPCIÓN DE SOLICITUDES ID23</t>
+  </si>
+  <si>
+    <t>RECEPCIÓN DE SOLICITUDES ID24</t>
+  </si>
+  <si>
+    <t>RECEPCIÓN DE SOLICITUDES ID25</t>
+  </si>
+  <si>
+    <t>RECEPCIÓN DE SOLICITUDES ID26</t>
+  </si>
+  <si>
+    <t>SOLUCION DE CASOS ID24</t>
+  </si>
+  <si>
+    <t>SOLUCION DE CASOS ID25</t>
+  </si>
+  <si>
+    <t>SOLUCION DE CASOS ID27</t>
+  </si>
+  <si>
+    <t>SOLUCION DE CASOS ID34</t>
+  </si>
+  <si>
+    <t>Planteamiento procedimiento de atención de requerimientos, soporte y mantenimiento @desarrolloanaliticapayc - revisión de par @desarrolloanaliticapayc - Recordar modificar procedimiento para que se almacenen los adjuntos resultado de la atención en un repositorio con carpetas por cada ID de solicitud</t>
+  </si>
+  <si>
+    <t>6. Modificar la metodología de revisión para que aparezcan los indicadores por cada aspecto en la tabla inicial para que el coordinador pueda aprobar o rechazar los paquetes de calificaciones mensuales, esto de acuerdo a una asignación previa del usuario obra</t>
+  </si>
+  <si>
+    <t>Documentar cada controlador de la aplicación en la wiki de la app</t>
+  </si>
+  <si>
+    <t>Actualizar formatos y rutina de cargue con los nuevos indicadores de comercial @desarrolloanaliticapayc</t>
+  </si>
+  <si>
+    <t>Modificación manual actualización de archivo indicadores en servidor</t>
+  </si>
+  <si>
+    <t>Revisión ID10</t>
+  </si>
+  <si>
+    <t>Creación de repositorios locales de Analitica</t>
   </si>
 </sst>
 </file>
@@ -279,11 +420,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +486,12 @@
       <color rgb="FF24272B"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -410,9 +557,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -450,7 +597,7 @@
     <xf numFmtId="21" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -467,8 +614,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -497,72 +644,13 @@
       <alignment horizontal="left" indent="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" indent="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" indent="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" indent="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1"/>
-    </dxf>
-    <dxf>
-      <protection locked="1"/>
-    </dxf>
-    <dxf>
-      <protection locked="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" indent="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" indent="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0" indent="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" readingOrder="0"/>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <alignment wrapText="1" readingOrder="0"/>
     </dxf>
@@ -639,7 +727,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -657,7 +745,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;_-;_-@_-"/>
+      <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -734,13 +822,13 @@
         <s v="Elaborar presentación de los resultados y presentar al área de tecnología"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="TIEMPO (días)" numFmtId="165">
+    <cacheField name="TIEMPO (días)" numFmtId="166">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.4467592592592594E-3" maxValue="0.95156249999999998"/>
     </cacheField>
     <cacheField name="TIEMPO (días laborables)" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.340277777777778E-3" maxValue="2.8546874999999998"/>
     </cacheField>
-    <cacheField name="FECHA" numFmtId="165">
+    <cacheField name="FECHA" numFmtId="166">
       <sharedItems count="4">
         <s v="2019-05-27 - 2019-06-02"/>
         <s v="2019-05-20 - 2019-05-26"/>
@@ -1123,7 +1211,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F52" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -1182,7 +1270,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" numFmtId="165" showAll="0"/>
+    <pivotField dataField="1" numFmtId="166" showAll="0"/>
     <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisCol" showAll="0">
       <items count="5">
@@ -1368,7 +1456,7 @@
     <dataField name="Suma de TIEMPO (días)" fld="3" baseField="2" baseItem="2"/>
   </dataFields>
   <formats count="20">
-    <format dxfId="39">
+    <format dxfId="19">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -1377,17 +1465,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -1397,17 +1485,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -1417,33 +1505,33 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="12">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -1453,17 +1541,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -1473,17 +1561,17 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="1" count="1" selected="0">
@@ -1504,15 +1592,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:F46" totalsRowShown="0">
-  <autoFilter ref="A1:F46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:F103" totalsRowShown="0">
+  <autoFilter ref="A1:F103"/>
   <tableColumns count="6">
     <tableColumn id="1" name="COLABORADOR"/>
     <tableColumn id="2" name="PROYECTO"/>
     <tableColumn id="3" name="ACTIVIDAD"/>
-    <tableColumn id="4" name="TIEMPO (días)" dataDxfId="41" dataCellStyle="Millares [0]"/>
+    <tableColumn id="4" name="TIEMPO (días)" dataDxfId="21" dataCellStyle="Millares [0]"/>
     <tableColumn id="5" name="TIEMPO (días laborables)"/>
-    <tableColumn id="6" name="FECHA" dataDxfId="40" dataCellStyle="Millares [0]"/>
+    <tableColumn id="6" name="FECHA" dataDxfId="20" dataCellStyle="Millares [0]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1783,7 +1871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -6032,10 +6120,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6964,6 +7052,1146 @@
         <v>0.51659722222222226</v>
       </c>
       <c r="F46" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="31">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E47">
+        <v>0.25</v>
+      </c>
+      <c r="F47" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="31">
+        <v>4.1712962962962959E-2</v>
+      </c>
+      <c r="E48">
+        <v>0.12513888888888888</v>
+      </c>
+      <c r="F48" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="31">
+        <v>0.10098379629629629</v>
+      </c>
+      <c r="E49">
+        <v>0.3029513888888889</v>
+      </c>
+      <c r="F49" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="31">
+        <v>0.19857638888888887</v>
+      </c>
+      <c r="E50">
+        <v>0.59572916666666664</v>
+      </c>
+      <c r="F50" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" s="31">
+        <v>0.13767361111111112</v>
+      </c>
+      <c r="E51">
+        <v>0.41302083333333339</v>
+      </c>
+      <c r="F51" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" s="31">
+        <v>0.41902777777777778</v>
+      </c>
+      <c r="E52">
+        <v>1.2570833333333333</v>
+      </c>
+      <c r="F52" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" s="31">
+        <v>6.6782407407407415E-3</v>
+      </c>
+      <c r="E53">
+        <v>2.0034722222222225E-2</v>
+      </c>
+      <c r="F53" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D54" s="31">
+        <v>0.22842592592592592</v>
+      </c>
+      <c r="E54">
+        <v>0.68527777777777776</v>
+      </c>
+      <c r="F54" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D55" s="31">
+        <v>4.1701388888888885E-2</v>
+      </c>
+      <c r="E55">
+        <v>0.12510416666666666</v>
+      </c>
+      <c r="F55" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" t="s">
+        <v>91</v>
+      </c>
+      <c r="D56" s="31">
+        <v>6.2083333333333331E-2</v>
+      </c>
+      <c r="E56">
+        <v>0.18625</v>
+      </c>
+      <c r="F56" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" s="31">
+        <v>0.12151620370370371</v>
+      </c>
+      <c r="E57">
+        <v>0.36454861111111114</v>
+      </c>
+      <c r="F57" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" t="s">
+        <v>92</v>
+      </c>
+      <c r="D58" s="31">
+        <v>0.38947916666666665</v>
+      </c>
+      <c r="E58">
+        <v>1.1684375</v>
+      </c>
+      <c r="F58" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" t="s">
+        <v>93</v>
+      </c>
+      <c r="D59" s="31">
+        <v>8.3622685185185189E-2</v>
+      </c>
+      <c r="E59">
+        <v>0.25086805555555558</v>
+      </c>
+      <c r="F59" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" t="s">
+        <v>82</v>
+      </c>
+      <c r="D60" s="31">
+        <v>5.6215277777777774E-2</v>
+      </c>
+      <c r="E60">
+        <v>0.16864583333333333</v>
+      </c>
+      <c r="F60" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" s="31">
+        <v>5.9722222222222225E-2</v>
+      </c>
+      <c r="E61">
+        <v>0.17916666666666667</v>
+      </c>
+      <c r="F61" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" t="s">
+        <v>95</v>
+      </c>
+      <c r="D62" s="31">
+        <v>0.10226851851851852</v>
+      </c>
+      <c r="E62">
+        <v>0.30680555555555555</v>
+      </c>
+      <c r="F62" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" t="s">
+        <v>85</v>
+      </c>
+      <c r="D63" s="31">
+        <v>5.7372685185185186E-2</v>
+      </c>
+      <c r="E63">
+        <v>0.17211805555555557</v>
+      </c>
+      <c r="F63" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" t="s">
+        <v>83</v>
+      </c>
+      <c r="C64" t="s">
+        <v>85</v>
+      </c>
+      <c r="D64" s="31">
+        <v>9.3344907407407404E-2</v>
+      </c>
+      <c r="E64">
+        <v>0.2800347222222222</v>
+      </c>
+      <c r="F64" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" t="s">
+        <v>96</v>
+      </c>
+      <c r="D65" s="31">
+        <v>5.2025462962962961E-2</v>
+      </c>
+      <c r="E65">
+        <v>0.15607638888888889</v>
+      </c>
+      <c r="F65" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>83</v>
+      </c>
+      <c r="C66" t="s">
+        <v>97</v>
+      </c>
+      <c r="D66" s="31">
+        <v>1.7326388888888888E-2</v>
+      </c>
+      <c r="E66">
+        <v>5.197916666666666E-2</v>
+      </c>
+      <c r="F66" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>83</v>
+      </c>
+      <c r="C67" t="s">
+        <v>98</v>
+      </c>
+      <c r="D67" s="31">
+        <v>1.2800925925925926E-2</v>
+      </c>
+      <c r="E67">
+        <v>3.8402777777777779E-2</v>
+      </c>
+      <c r="F67" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" t="s">
+        <v>86</v>
+      </c>
+      <c r="C68" t="s">
+        <v>99</v>
+      </c>
+      <c r="D68" s="31">
+        <v>2.7951388888888887E-2</v>
+      </c>
+      <c r="E68">
+        <v>8.385416666666666E-2</v>
+      </c>
+      <c r="F68" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" t="s">
+        <v>87</v>
+      </c>
+      <c r="D69" s="31">
+        <v>2.9629629629629627E-2</v>
+      </c>
+      <c r="E69">
+        <v>8.8888888888888878E-2</v>
+      </c>
+      <c r="F69" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" t="s">
+        <v>88</v>
+      </c>
+      <c r="C70" t="s">
+        <v>100</v>
+      </c>
+      <c r="D70" s="31">
+        <v>6.1342592592592594E-2</v>
+      </c>
+      <c r="E70">
+        <v>0.18402777777777779</v>
+      </c>
+      <c r="F70" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" t="s">
+        <v>88</v>
+      </c>
+      <c r="C71" t="s">
+        <v>101</v>
+      </c>
+      <c r="D71" s="31">
+        <v>5.7870370370370371E-2</v>
+      </c>
+      <c r="E71">
+        <v>0.1736111111111111</v>
+      </c>
+      <c r="F71" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>65</v>
+      </c>
+      <c r="B72" t="s">
+        <v>88</v>
+      </c>
+      <c r="C72" t="s">
+        <v>102</v>
+      </c>
+      <c r="D72" s="31">
+        <v>9.6064814814814808E-4</v>
+      </c>
+      <c r="E72">
+        <v>2.8819444444444444E-3</v>
+      </c>
+      <c r="F72" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>65</v>
+      </c>
+      <c r="B73" t="s">
+        <v>88</v>
+      </c>
+      <c r="C73" t="s">
+        <v>103</v>
+      </c>
+      <c r="D73" s="31">
+        <v>2.7141203703703706E-2</v>
+      </c>
+      <c r="E73">
+        <v>8.1423611111111113E-2</v>
+      </c>
+      <c r="F73" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>65</v>
+      </c>
+      <c r="B74" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74" t="s">
+        <v>104</v>
+      </c>
+      <c r="D74" s="31">
+        <v>1.292824074074074E-2</v>
+      </c>
+      <c r="E74">
+        <v>3.878472222222222E-2</v>
+      </c>
+      <c r="F74" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>65</v>
+      </c>
+      <c r="B75" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" t="s">
+        <v>105</v>
+      </c>
+      <c r="D75" s="31">
+        <v>0.24208333333333334</v>
+      </c>
+      <c r="E75">
+        <v>0.72625000000000006</v>
+      </c>
+      <c r="F75" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>65</v>
+      </c>
+      <c r="B76" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" t="s">
+        <v>106</v>
+      </c>
+      <c r="D76" s="31">
+        <v>5.1724537037037034E-2</v>
+      </c>
+      <c r="E76">
+        <v>0.15517361111111111</v>
+      </c>
+      <c r="F76" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>65</v>
+      </c>
+      <c r="B77" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" t="s">
+        <v>107</v>
+      </c>
+      <c r="D77" s="31">
+        <v>8.0254629629629634E-2</v>
+      </c>
+      <c r="E77">
+        <v>0.24076388888888889</v>
+      </c>
+      <c r="F77" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>65</v>
+      </c>
+      <c r="B78" t="s">
+        <v>23</v>
+      </c>
+      <c r="C78" t="s">
+        <v>108</v>
+      </c>
+      <c r="D78" s="31">
+        <v>1.0243055555555556E-2</v>
+      </c>
+      <c r="E78">
+        <v>3.0729166666666669E-2</v>
+      </c>
+      <c r="F78" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>65</v>
+      </c>
+      <c r="B79" t="s">
+        <v>23</v>
+      </c>
+      <c r="C79" t="s">
+        <v>109</v>
+      </c>
+      <c r="D79" s="31">
+        <v>2.6909722222222224E-2</v>
+      </c>
+      <c r="E79">
+        <v>8.0729166666666671E-2</v>
+      </c>
+      <c r="F79" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>65</v>
+      </c>
+      <c r="B80" t="s">
+        <v>23</v>
+      </c>
+      <c r="C80" t="s">
+        <v>110</v>
+      </c>
+      <c r="D80" s="31">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E80">
+        <v>0.25</v>
+      </c>
+      <c r="F80" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>65</v>
+      </c>
+      <c r="B81" t="s">
+        <v>23</v>
+      </c>
+      <c r="C81" t="s">
+        <v>111</v>
+      </c>
+      <c r="D81" s="31">
+        <v>0.10964120370370371</v>
+      </c>
+      <c r="E81">
+        <v>0.32892361111111112</v>
+      </c>
+      <c r="F81" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>65</v>
+      </c>
+      <c r="B82" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" t="s">
+        <v>112</v>
+      </c>
+      <c r="D82" s="31">
+        <v>5.4560185185185184E-2</v>
+      </c>
+      <c r="E82">
+        <v>0.16368055555555555</v>
+      </c>
+      <c r="F82" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>65</v>
+      </c>
+      <c r="B83" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" t="s">
+        <v>113</v>
+      </c>
+      <c r="D83" s="31">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E83">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F83" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>65</v>
+      </c>
+      <c r="B84" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" t="s">
+        <v>114</v>
+      </c>
+      <c r="D84" s="31">
+        <v>2.462962962962963E-2</v>
+      </c>
+      <c r="E84">
+        <v>7.3888888888888893E-2</v>
+      </c>
+      <c r="F84" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>65</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" t="s">
+        <v>115</v>
+      </c>
+      <c r="D85" s="31">
+        <v>1.2546296296296297E-2</v>
+      </c>
+      <c r="E85">
+        <v>3.7638888888888888E-2</v>
+      </c>
+      <c r="F85" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>65</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" t="s">
+        <v>116</v>
+      </c>
+      <c r="D86" s="31">
+        <v>5.6250000000000001E-2</v>
+      </c>
+      <c r="E86">
+        <v>0.16875000000000001</v>
+      </c>
+      <c r="F86" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>65</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" t="s">
+        <v>117</v>
+      </c>
+      <c r="D87" s="31">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E87">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F87" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>65</v>
+      </c>
+      <c r="B88" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88" t="s">
+        <v>118</v>
+      </c>
+      <c r="D88" s="31">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E88">
+        <v>0.125</v>
+      </c>
+      <c r="F88" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>65</v>
+      </c>
+      <c r="B89" t="s">
+        <v>3</v>
+      </c>
+      <c r="C89" t="s">
+        <v>119</v>
+      </c>
+      <c r="D89" s="31">
+        <v>1.9386574074074073E-2</v>
+      </c>
+      <c r="E89">
+        <v>5.8159722222222224E-2</v>
+      </c>
+      <c r="F89" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>65</v>
+      </c>
+      <c r="B90" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" t="s">
+        <v>82</v>
+      </c>
+      <c r="D90" s="31">
+        <v>9.6898148148148164E-2</v>
+      </c>
+      <c r="E90">
+        <v>0.29069444444444448</v>
+      </c>
+      <c r="F90" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>65</v>
+      </c>
+      <c r="B91" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91" t="s">
+        <v>120</v>
+      </c>
+      <c r="D91" s="31">
+        <v>9.2372685185185197E-2</v>
+      </c>
+      <c r="E91">
+        <v>0.27711805555555558</v>
+      </c>
+      <c r="F91" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>65</v>
+      </c>
+      <c r="B92" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92" t="s">
+        <v>94</v>
+      </c>
+      <c r="D92" s="31">
+        <v>2.4421296296296292E-2</v>
+      </c>
+      <c r="E92">
+        <v>7.3263888888888878E-2</v>
+      </c>
+      <c r="F92" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>65</v>
+      </c>
+      <c r="B93" t="s">
+        <v>88</v>
+      </c>
+      <c r="C93" t="s">
+        <v>121</v>
+      </c>
+      <c r="D93" s="31">
+        <v>0.59833333333333327</v>
+      </c>
+      <c r="E93">
+        <v>1.7949999999999999</v>
+      </c>
+      <c r="F93" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>65</v>
+      </c>
+      <c r="B94" t="s">
+        <v>88</v>
+      </c>
+      <c r="C94" t="s">
+        <v>122</v>
+      </c>
+      <c r="D94" s="31">
+        <v>8.7615740740740744E-3</v>
+      </c>
+      <c r="E94">
+        <v>2.6284722222222223E-2</v>
+      </c>
+      <c r="F94" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>65</v>
+      </c>
+      <c r="B95" t="s">
+        <v>23</v>
+      </c>
+      <c r="C95" t="s">
+        <v>123</v>
+      </c>
+      <c r="D95" s="31">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E95">
+        <v>0.25</v>
+      </c>
+      <c r="F95" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>65</v>
+      </c>
+      <c r="B96" t="s">
+        <v>23</v>
+      </c>
+      <c r="C96" t="s">
+        <v>124</v>
+      </c>
+      <c r="D96" s="31">
+        <v>1.4606481481481482E-2</v>
+      </c>
+      <c r="E96">
+        <v>4.3819444444444446E-2</v>
+      </c>
+      <c r="F96" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>65</v>
+      </c>
+      <c r="B97" t="s">
+        <v>23</v>
+      </c>
+      <c r="C97" t="s">
+        <v>125</v>
+      </c>
+      <c r="D97" s="31">
+        <v>4.1770833333333333E-2</v>
+      </c>
+      <c r="E97">
+        <v>0.12531249999999999</v>
+      </c>
+      <c r="F97" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>65</v>
+      </c>
+      <c r="B98" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" t="s">
+        <v>126</v>
+      </c>
+      <c r="D98" s="31">
+        <v>4.8275462962962958E-2</v>
+      </c>
+      <c r="E98">
+        <v>0.14482638888888888</v>
+      </c>
+      <c r="F98" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>65</v>
+      </c>
+      <c r="B99" t="s">
+        <v>23</v>
+      </c>
+      <c r="C99" t="s">
+        <v>106</v>
+      </c>
+      <c r="D99" s="31">
+        <v>5.1724537037037034E-2</v>
+      </c>
+      <c r="E99">
+        <v>0.15517361111111111</v>
+      </c>
+      <c r="F99" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>65</v>
+      </c>
+      <c r="B100" t="s">
+        <v>23</v>
+      </c>
+      <c r="C100" t="s">
+        <v>107</v>
+      </c>
+      <c r="D100" s="31">
+        <v>8.0254629629629634E-2</v>
+      </c>
+      <c r="E100">
+        <v>0.24076388888888889</v>
+      </c>
+      <c r="F100" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>65</v>
+      </c>
+      <c r="B101" t="s">
+        <v>23</v>
+      </c>
+      <c r="C101" t="s">
+        <v>108</v>
+      </c>
+      <c r="D101" s="31">
+        <v>1.0243055555555556E-2</v>
+      </c>
+      <c r="E101">
+        <v>3.0729166666666669E-2</v>
+      </c>
+      <c r="F101" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>65</v>
+      </c>
+      <c r="B102" t="s">
+        <v>23</v>
+      </c>
+      <c r="C102" t="s">
+        <v>109</v>
+      </c>
+      <c r="D102" s="31">
+        <v>2.6909722222222224E-2</v>
+      </c>
+      <c r="E102">
+        <v>8.0729166666666671E-2</v>
+      </c>
+      <c r="F102" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>65</v>
+      </c>
+      <c r="B103" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103" t="s">
+        <v>111</v>
+      </c>
+      <c r="D103" s="31">
+        <v>0.10964120370370371</v>
+      </c>
+      <c r="E103">
+        <v>0.32892361111111112</v>
+      </c>
+      <c r="F103" s="31" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>